<commit_message>
Add ignore Index option
</commit_message>
<xml_diff>
--- a/Assignment_2/Question_5/통합자료.xlsx
+++ b/Assignment_2/Question_5/통합자료.xlsx
@@ -528,7 +528,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -554,7 +554,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -658,7 +658,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>

</xml_diff>